<commit_message>
updating the start year in Scen__ForLCOE.xlsx to 2025
The model is infeasible with a start in 2020 (techs start year is 2025)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen__ForLCOE.xlsx
+++ b/SuppXLS/Scen__ForLCOE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40A21D6F-438E-472C-981C-3745CCD12CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1648F13-0FE2-46AC-B218-48445847D1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
+    <workbookView xWindow="-3564" yWindow="-14184" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
@@ -495,7 +495,7 @@
   <dimension ref="C5:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -555,7 +555,7 @@
         <v>12</v>
       </c>
       <c r="F7" s="1">
-        <v>2020</v>
+        <v>2025</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Restricting the activity bound to power since it conflicts with some UCs for hydro in some regions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen__ForLCOE.xlsx
+++ b/SuppXLS/Scen__ForLCOE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1648F13-0FE2-46AC-B218-48445847D1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5B4293-4311-43DD-A470-946E44D5B59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3564" yWindow="-14184" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
+    <workbookView xWindow="1980" yWindow="-12756" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
@@ -34,6 +34,41 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mahmoud Mobir</author>
+  </authors>
+  <commentList>
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{A104A450-46BF-4EA4-93C7-C4A97397BA9A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahmoud Mobir:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+12-8-2021
+This was 2020 but it caused infeasiblities. Made it 2025. </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
@@ -82,9 +117,6 @@
     <t>ELE</t>
   </si>
   <si>
-    <t>EN*</t>
-  </si>
-  <si>
     <t>The INS table imposes very small activity bounds on all the power plants of the model</t>
   </si>
   <si>
@@ -92,13 +124,16 @@
   </si>
   <si>
     <t>The objective is to to be able to see why CCS doesn't deploy under high carbon prices scenarios</t>
+  </si>
+  <si>
+    <t>EN_Z*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +151,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -472,17 +520,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -491,11 +539,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6E33AC-1F00-408E-86F9-2FC33A587035}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6E33AC-1F00-408E-86F9-2FC33A587035}">
   <dimension ref="C5:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -562,14 +610,14 @@
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="1">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="3:12" x14ac:dyDescent="0.3">
@@ -595,7 +643,7 @@
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="3:12" x14ac:dyDescent="0.3">
@@ -621,10 +669,11 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding 2080 to the lcoe table
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen__ForLCOE.xlsx
+++ b/SuppXLS/Scen__ForLCOE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A5B4293-4311-43DD-A470-946E44D5B59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97290066-031A-440C-BB85-99645EF1A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="-12756" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -540,10 +540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6E33AC-1F00-408E-86F9-2FC33A587035}">
-  <dimension ref="C5:L9"/>
+  <dimension ref="C5:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -655,7 +655,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="1">
-        <v>0</v>
+        <v>2080</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>13</v>
@@ -669,6 +669,31 @@
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="1">
+        <v>1</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding DAC to the lcoe table
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen__ForLCOE.xlsx
+++ b/SuppXLS/Scen__ForLCOE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda_models\IEMM_v60_10-1\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97290066-031A-440C-BB85-99645EF1A44A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C14101B-8BBF-423E-ABC0-EB69FCCDB165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="-12756" windowWidth="17280" windowHeight="10044" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
+    <workbookView xWindow="372" yWindow="3360" windowWidth="24888" windowHeight="9696" activeTab="1" xr2:uid="{026F1D9E-4EED-4403-96EC-84BE73EA0A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="3" r:id="rId1"/>
@@ -65,12 +65,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{C2F9806E-80B5-4C1E-8A25-3702987A6284}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mahmoud Mobir:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+12-8-2021
+This was 2020 but it caused infeasiblities. Made it 2025. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="20">
   <si>
     <t>~TFM_INS</t>
   </si>
@@ -127,6 +152,9 @@
   </si>
   <si>
     <t>EN_Z*</t>
+  </si>
+  <si>
+    <t>SNK_DAC</t>
   </si>
 </sst>
 </file>
@@ -540,13 +568,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6E33AC-1F00-408E-86F9-2FC33A587035}">
-  <dimension ref="C5:L10"/>
+  <dimension ref="C5:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="5" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
@@ -697,6 +728,98 @@
         <v>18</v>
       </c>
     </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="1">
+        <v>2025</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>2050</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="1">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="1">
+        <v>2080</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="D14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="1">
+        <v>1</v>
+      </c>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>